<commit_message>
Made new branch for part. Added files
</commit_message>
<xml_diff>
--- a/DB/GradesDatabase-goldenversion.xlsx
+++ b/DB/GradesDatabase-goldenversion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
   <si>
     <t>NAME</t>
   </si>
@@ -198,12 +198,19 @@
   <si>
     <t>ID</t>
   </si>
+  <si>
+    <t>PROJECT 4</t>
+  </si>
+  <si>
+    <t>ASSIGNMENT 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -267,6 +274,16 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="3">
@@ -411,7 +428,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -466,6 +483,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -835,13 +854,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.5" customWidth="1"/>
-    <col min="6" max="6" width="4.5" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="17" width="19.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="2.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="7.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" customHeight="1">
@@ -1199,12 +1218,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" customHeight="1">
@@ -1319,8 +1338,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.83203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
@@ -1456,7 +1475,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
@@ -1464,10 +1483,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
@@ -1483,6 +1502,9 @@
       <c r="D1" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="E1" s="19" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1497,6 +1519,9 @@
       <c r="D2" s="2">
         <v>75</v>
       </c>
+      <c r="E2" t="n">
+        <v>95.0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1511,6 +1536,9 @@
       <c r="D3" s="2">
         <v>71</v>
       </c>
+      <c r="E3" t="n">
+        <v>96.0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -1525,6 +1553,9 @@
       <c r="D4" s="2">
         <v>85</v>
       </c>
+      <c r="E4" t="n">
+        <v>65.0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -1539,6 +1570,9 @@
       <c r="D5" s="2">
         <v>40</v>
       </c>
+      <c r="E5" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -1553,6 +1587,9 @@
       <c r="D6" s="2">
         <v>90</v>
       </c>
+      <c r="E6" t="n">
+        <v>87.0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -1567,6 +1604,9 @@
       <c r="D7" s="2">
         <v>85</v>
       </c>
+      <c r="E7" t="n">
+        <v>65.0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -1581,6 +1621,9 @@
       <c r="D8" s="2">
         <v>85</v>
       </c>
+      <c r="E8" t="n">
+        <v>90.0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="28.5" customHeight="1">
       <c r="A9" s="2" t="s">
@@ -1595,6 +1638,9 @@
       <c r="D9" s="2">
         <v>100</v>
       </c>
+      <c r="E9" t="n">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" customHeight="1">
       <c r="A10" s="2" t="s">
@@ -1609,6 +1655,9 @@
       <c r="D10" s="2">
         <v>75</v>
       </c>
+      <c r="E10" t="n">
+        <v>67.0</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="28.5" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -1623,6 +1672,9 @@
       <c r="D11" s="2">
         <v>71</v>
       </c>
+      <c r="E11" t="n">
+        <v>95.0</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="28.5" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -1637,6 +1689,9 @@
       <c r="D12" s="2">
         <v>85</v>
       </c>
+      <c r="E12" t="n">
+        <v>96.0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" customHeight="1">
       <c r="A13" s="2" t="s">
@@ -1651,6 +1706,9 @@
       <c r="D13" s="2">
         <v>40</v>
       </c>
+      <c r="E13" t="n">
+        <v>65.0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="28.5" customHeight="1">
       <c r="A14" s="2" t="s">
@@ -1665,6 +1723,9 @@
       <c r="D14" s="2">
         <v>90</v>
       </c>
+      <c r="E14" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="28.5" customHeight="1">
       <c r="A15" s="2" t="s">
@@ -1678,6 +1739,9 @@
       </c>
       <c r="D15" s="2">
         <v>85</v>
+      </c>
+      <c r="E15" t="n">
+        <v>87.0</v>
       </c>
     </row>
   </sheetData>
@@ -1693,7 +1757,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -1702,9 +1766,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
@@ -1720,6 +1784,9 @@
       <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
+      <c r="E1" s="18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1729,6 +1796,9 @@
         <v>83</v>
       </c>
       <c r="C2" s="3"/>
+      <c r="D2" t="n">
+        <v>95.0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1738,6 +1808,9 @@
         <v>87</v>
       </c>
       <c r="C3" s="3"/>
+      <c r="D3" t="n">
+        <v>96.0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -1747,6 +1820,9 @@
         <v>84</v>
       </c>
       <c r="C4" s="3"/>
+      <c r="D4" t="n">
+        <v>65.0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -1756,6 +1832,9 @@
         <v>91</v>
       </c>
       <c r="C5" s="3"/>
+      <c r="D5" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -1765,6 +1844,9 @@
         <v>100</v>
       </c>
       <c r="C6" s="3"/>
+      <c r="D6" t="n">
+        <v>87.0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -1779,6 +1861,9 @@
       <c r="D7">
         <v>89</v>
       </c>
+      <c r="E7" t="n">
+        <v>65.0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -1793,6 +1878,9 @@
       <c r="D8">
         <v>92</v>
       </c>
+      <c r="E8" t="n">
+        <v>90.0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="28.5" customHeight="1">
       <c r="A9" s="2" t="s">
@@ -1807,6 +1895,9 @@
       <c r="D9">
         <v>50</v>
       </c>
+      <c r="E9" t="n">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" customHeight="1">
       <c r="A10" s="2" t="s">
@@ -1820,6 +1911,9 @@
       </c>
       <c r="D10">
         <v>93</v>
+      </c>
+      <c r="E10" t="n">
+        <v>67.0</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.5" customHeight="1">
@@ -1923,10 +2017,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">

</xml_diff>

<commit_message>
Reset Grades database excel file
</commit_message>
<xml_diff>
--- a/DB/GradesDatabase-goldenversion.xlsx
+++ b/DB/GradesDatabase-goldenversion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="54">
   <si>
     <t>NAME</t>
   </si>
@@ -198,19 +198,12 @@
   <si>
     <t>ID</t>
   </si>
-  <si>
-    <t>PROJECT 4</t>
-  </si>
-  <si>
-    <t>ASSIGNMENT 4</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -274,16 +267,6 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
     </font>
   </fonts>
   <fills count="3">
@@ -428,7 +411,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -483,8 +466,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -854,13 +835,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="17" width="19.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="2.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="7.5" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="17" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="4.5" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" customHeight="1">
@@ -1218,12 +1199,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" customHeight="1">
@@ -1338,8 +1319,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
@@ -1475,7 +1456,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
@@ -1483,10 +1464,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
@@ -1502,9 +1483,6 @@
       <c r="D1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1519,9 +1497,6 @@
       <c r="D2" s="2">
         <v>75</v>
       </c>
-      <c r="E2" t="n">
-        <v>95.0</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1536,9 +1511,6 @@
       <c r="D3" s="2">
         <v>71</v>
       </c>
-      <c r="E3" t="n">
-        <v>96.0</v>
-      </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -1553,9 +1525,6 @@
       <c r="D4" s="2">
         <v>85</v>
       </c>
-      <c r="E4" t="n">
-        <v>65.0</v>
-      </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -1570,9 +1539,6 @@
       <c r="D5" s="2">
         <v>40</v>
       </c>
-      <c r="E5" t="n">
-        <v>17.0</v>
-      </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -1587,9 +1553,6 @@
       <c r="D6" s="2">
         <v>90</v>
       </c>
-      <c r="E6" t="n">
-        <v>87.0</v>
-      </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -1604,9 +1567,6 @@
       <c r="D7" s="2">
         <v>85</v>
       </c>
-      <c r="E7" t="n">
-        <v>65.0</v>
-      </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -1621,9 +1581,6 @@
       <c r="D8" s="2">
         <v>85</v>
       </c>
-      <c r="E8" t="n">
-        <v>90.0</v>
-      </c>
     </row>
     <row r="9" spans="1:4" ht="28.5" customHeight="1">
       <c r="A9" s="2" t="s">
@@ -1638,9 +1595,6 @@
       <c r="D9" s="2">
         <v>100</v>
       </c>
-      <c r="E9" t="n">
-        <v>35.0</v>
-      </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" customHeight="1">
       <c r="A10" s="2" t="s">
@@ -1655,9 +1609,6 @@
       <c r="D10" s="2">
         <v>75</v>
       </c>
-      <c r="E10" t="n">
-        <v>67.0</v>
-      </c>
     </row>
     <row r="11" spans="1:4" ht="28.5" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -1672,9 +1623,6 @@
       <c r="D11" s="2">
         <v>71</v>
       </c>
-      <c r="E11" t="n">
-        <v>95.0</v>
-      </c>
     </row>
     <row r="12" spans="1:4" ht="28.5" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -1689,9 +1637,6 @@
       <c r="D12" s="2">
         <v>85</v>
       </c>
-      <c r="E12" t="n">
-        <v>96.0</v>
-      </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" customHeight="1">
       <c r="A13" s="2" t="s">
@@ -1706,9 +1651,6 @@
       <c r="D13" s="2">
         <v>40</v>
       </c>
-      <c r="E13" t="n">
-        <v>65.0</v>
-      </c>
     </row>
     <row r="14" spans="1:4" ht="28.5" customHeight="1">
       <c r="A14" s="2" t="s">
@@ -1723,9 +1665,6 @@
       <c r="D14" s="2">
         <v>90</v>
       </c>
-      <c r="E14" t="n">
-        <v>17.0</v>
-      </c>
     </row>
     <row r="15" spans="1:4" ht="28.5" customHeight="1">
       <c r="A15" s="2" t="s">
@@ -1739,9 +1678,6 @@
       </c>
       <c r="D15" s="2">
         <v>85</v>
-      </c>
-      <c r="E15" t="n">
-        <v>87.0</v>
       </c>
     </row>
   </sheetData>
@@ -1757,7 +1693,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -1766,9 +1702,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
@@ -1784,9 +1720,6 @@
       <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1796,9 +1729,6 @@
         <v>83</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="E2" t="n">
-        <v>95.0</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1808,9 +1738,6 @@
         <v>87</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="E3" t="n">
-        <v>96.0</v>
-      </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -1820,9 +1747,6 @@
         <v>84</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="E4" t="n">
-        <v>65.0</v>
-      </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -1832,9 +1756,6 @@
         <v>91</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="E5" t="n">
-        <v>17.0</v>
-      </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -1844,9 +1765,6 @@
         <v>100</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="E6" t="n">
-        <v>87.0</v>
-      </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -1861,9 +1779,6 @@
       <c r="D7">
         <v>89</v>
       </c>
-      <c r="E7" t="n">
-        <v>65.0</v>
-      </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -1878,9 +1793,6 @@
       <c r="D8">
         <v>92</v>
       </c>
-      <c r="E8" t="n">
-        <v>90.0</v>
-      </c>
     </row>
     <row r="9" spans="1:4" ht="28.5" customHeight="1">
       <c r="A9" s="2" t="s">
@@ -1895,9 +1807,6 @@
       <c r="D9">
         <v>50</v>
       </c>
-      <c r="E9" t="n">
-        <v>35.0</v>
-      </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" customHeight="1">
       <c r="A10" s="2" t="s">
@@ -1912,9 +1821,6 @@
       <c r="D10">
         <v>93</v>
       </c>
-      <c r="E10" t="n">
-        <v>67.0</v>
-      </c>
     </row>
     <row r="11" spans="1:4" ht="28.5" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -1929,9 +1835,6 @@
       <c r="D11">
         <v>99</v>
       </c>
-      <c r="E11" t="n">
-        <v>87.0</v>
-      </c>
     </row>
     <row r="12" spans="1:4" ht="28.5" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -1946,9 +1849,6 @@
       <c r="D12">
         <v>87</v>
       </c>
-      <c r="E12" t="n">
-        <v>65.0</v>
-      </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" customHeight="1">
       <c r="A13" s="2" t="s">
@@ -1963,9 +1863,6 @@
       <c r="D13">
         <v>98</v>
       </c>
-      <c r="E13" t="n">
-        <v>90.0</v>
-      </c>
     </row>
     <row r="14" spans="1:4" ht="28.5" customHeight="1">
       <c r="A14" s="2" t="s">
@@ -1980,9 +1877,6 @@
       <c r="D14">
         <v>90</v>
       </c>
-      <c r="E14" t="n">
-        <v>35.0</v>
-      </c>
     </row>
     <row r="15" spans="1:4" ht="28.5" customHeight="1">
       <c r="A15" s="2" t="s">
@@ -1996,9 +1890,6 @@
       </c>
       <c r="D15">
         <v>95</v>
-      </c>
-      <c r="E15" t="n">
-        <v>67.0</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.5" customHeight="1">
@@ -2032,10 +1923,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.1640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">

</xml_diff>